<commit_message>
1. Added new data type "color" 2. Fix the Import file after adding color data type 3. Fix the image upload after import excel
</commit_message>
<xml_diff>
--- a/excel sample/sample.xlsx
+++ b/excel sample/sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>123qwd</t>
   </si>
@@ -45,6 +45,57 @@
   </si>
   <si>
     <t>Handicraft</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>wood type</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>asdasdasa</t>
+  </si>
+  <si>
+    <t>Outdoor</t>
+  </si>
+  <si>
+    <t>Tiger wood</t>
+  </si>
+  <si>
+    <t>Aqua</t>
   </si>
 </sst>
 </file>
@@ -120,15 +171,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1304925</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1212303</xdr:rowOff>
+      <xdr:colOff>1266825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1250403</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -151,7 +202,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="781050" y="1238250"/>
+          <a:off x="742950" y="1876425"/>
           <a:ext cx="1133475" cy="1126578"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -165,13 +216,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1190625</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>1057275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -197,6 +248,50 @@
         <a:xfrm>
           <a:off x="809625" y="66675"/>
           <a:ext cx="990600" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1266825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="3352800"/>
+          <a:ext cx="1162050" cy="1162050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -471,85 +566,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L5"/>
+  <dimension ref="B1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1">
-        <v>1</v>
-      </c>
-      <c r="I1" s="1">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1">
-        <v>1</v>
-      </c>
-      <c r="K1" s="1">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1"/>
+    <row r="1" spans="2:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" spans="2:12" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1">
+        <v>213123</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>2</v>
-      </c>
-      <c r="I2" s="1">
-        <v>2</v>
-      </c>
-      <c r="J2" s="1">
-        <v>2</v>
-      </c>
-      <c r="K2" s="1">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1">
-        <v>2</v>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="1">
+        <v>133312</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="117.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:12" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1">
+        <v>1122</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2222</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
change the thead from depth to length
</commit_message>
<xml_diff>
--- a/excel sample/sample.xlsx
+++ b/excel sample/sample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Inventory\excel sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F96DA5C-DD02-4E4E-B244-C997CC45B0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -71,9 +72,6 @@
     <t>stock</t>
   </si>
   <si>
-    <t>depth</t>
-  </si>
-  <si>
     <t>color</t>
   </si>
   <si>
@@ -96,12 +94,15 @@
   </si>
   <si>
     <t>Aqua</t>
+  </si>
+  <si>
+    <t>length</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,7 +184,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -227,7 +234,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -271,7 +284,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -565,11 +584,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +620,7 @@
         <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s">
         <v>13</v>
@@ -610,10 +629,10 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
         <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="2:12" ht="99" customHeight="1" x14ac:dyDescent="0.25">
@@ -643,7 +662,7 @@
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2" s="1">
         <v>213123</v>
@@ -676,7 +695,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L3" s="1">
         <v>133312</v>
@@ -688,28 +707,28 @@
         <v>1122</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2</v>
-      </c>
-      <c r="H4" s="1">
-        <v>2</v>
-      </c>
-      <c r="I4" s="1">
-        <v>2</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="L4" s="1">
         <v>2222</v>

</xml_diff>